<commit_message>
importando tasktickapp p controlador
</commit_message>
<xml_diff>
--- a/BD_TaskTick.xlsx
+++ b/BD_TaskTick.xlsx
@@ -1,79 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\17 - Freelance\6 - TaskTick\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4227A3EA-D885-4C87-AF28-45FE5C2EBF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr codeName="EstaPastaDeTrabalho"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3A2650AF-A382-4D48-98EC-FC65D117397C}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Atividades" sheetId="1" r:id="rId1"/>
-    <sheet name="Horas Trabalhadas" sheetId="2" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Atividades" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Horas Trabalhadas" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Projeto</t>
-  </si>
-  <si>
-    <t>Descrição</t>
-  </si>
-  <si>
-    <t>Cliente</t>
-  </si>
-  <si>
-    <t>Atividade</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Hora Início</t>
-  </si>
-  <si>
-    <t>Hora Fim</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -92,44 +47,103 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D030D705-8D31-4936-B7B5-8D7B9AF2B103}" name="Tabela2" displayName="Tabela2" ref="A1:C2" totalsRowShown="0">
-  <autoFilter ref="A1:C2" xr:uid="{D030D705-8D31-4936-B7B5-8D7B9AF2B103}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela2" displayName="Tabela2" ref="A1:C2" headerRowCount="1" totalsRowShown="0">
+  <autoFilter ref="A1:C2"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{DDE21B1D-400E-49CA-AAB1-F4CC13218DBA}" name="Projeto"/>
-    <tableColumn id="2" xr3:uid="{9F33E76D-90D0-4744-A0E2-591C8B1DA458}" name="Descrição"/>
-    <tableColumn id="3" xr3:uid="{D98A8FF2-6E6B-4C98-A316-022BB6A77166}" name="Cliente"/>
+    <tableColumn id="1" name="Projeto"/>
+    <tableColumn id="2" name="Descrição"/>
+    <tableColumn id="3" name="Cliente"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0BF09A6B-2330-458B-BB1D-9641C1C6C609}" name="Tabela1" displayName="Tabela1" ref="A1:D2" totalsRowShown="0">
-  <autoFilter ref="A1:D2" xr:uid="{0BF09A6B-2330-458B-BB1D-9641C1C6C609}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela1" displayName="Tabela1" ref="A1:D2" headerRowCount="1" totalsRowShown="0">
+  <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{98F5C062-1092-45C4-9BCD-593F1B19ED3D}" name="Atividade"/>
-    <tableColumn id="2" xr3:uid="{E15B2175-4F17-4392-9F88-34AAEBF7AFAE}" name="Data"/>
-    <tableColumn id="3" xr3:uid="{F281588B-A80D-490E-AB9B-95DABEAF96BF}" name="Hora Início"/>
-    <tableColumn id="4" xr3:uid="{043D7A26-11B7-485A-972F-2E5BF2507BBB}" name="Hora Fim"/>
+    <tableColumn id="1" name="Atividade"/>
+    <tableColumn id="2" name="Data"/>
+    <tableColumn id="3" name="Hora Início"/>
+    <tableColumn id="4" name="Hora Fim"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -431,73 +445,93 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B98E73E5-49F1-4E79-80AB-1556765F28F0}">
-  <sheetPr codeName="Planilha1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Planilha1">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col width="9.109375" customWidth="1" min="1" max="1"/>
+    <col width="10.88671875" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Projeto</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Descrição</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Cliente</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9B5D24-3752-4976-BFAD-31C0E2555612}">
-  <sheetPr codeName="Planilha2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Planilha2">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="A1" sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col width="10.88671875" customWidth="1" min="1" max="1"/>
+    <col width="11.88671875" customWidth="1" min="3" max="3"/>
+    <col width="10.33203125" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Atividade</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Data</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Hora Início</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Hora Fim</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Alterações em models.py - revisão geral
</commit_message>
<xml_diff>
--- a/BD_TaskTick.xlsx
+++ b/BD_TaskTick.xlsx
@@ -1,41 +1,69 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Atividades" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Horas Trabalhadas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Atividade</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Hora Início</t>
+  </si>
+  <si>
+    <t>Hora Fim</t>
+  </si>
+  <si>
+    <t>TASKTICK</t>
+  </si>
+  <si>
+    <t>7/17/24</t>
+  </si>
+  <si>
+    <t>07:00</t>
+  </si>
+  <si>
+    <t>09:00</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -69,83 +97,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -433,85 +394,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Projeto</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Descrição</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Cliente</t>
-        </is>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>teste 1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">teste 2 </t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>teste 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Sistema ICAN</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Projeto para gerenciamento de cadastro de beneficiários</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>ICAN</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>TESTE</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>TESTE DESCRIÇÃO</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>TESTE CLIENTE</t>
-        </is>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
alteracoes para carregar combobox
</commit_message>
<xml_diff>
--- a/BD_TaskTick.xlsx
+++ b/BD_TaskTick.xlsx
@@ -1,75 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Horas Trabalhadas" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Atividades" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Horas Trabalhadas" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Atividade</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Hora Início</t>
-  </si>
-  <si>
-    <t>Hora Fim</t>
-  </si>
-  <si>
-    <t>TASKTICK</t>
-  </si>
-  <si>
-    <t>7/17/24</t>
-  </si>
-  <si>
-    <t>07:00</t>
-  </si>
-  <si>
-    <t>09:00</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -92,21 +65,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -394,42 +443,235 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Projeto</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Descrição</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Cliente</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Registro de Auto Controle - Art Coating</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Registro das informações de produção</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Art Coating</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Sistema de ordens de serviço de manutenção</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Gerenciamento das ordens de manutenção</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Art Coating</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Sistema ICAN</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Gerenciamento de beneficiários</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Instituto cultural de artes nobres</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>SISTEMA TESTE</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>teste descrição</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>teste cliente 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>testetstete</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>fsfs</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>sfdfs</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="38.33203125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="7.5546875" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="10" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="8.44140625" bestFit="1" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Atividade</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Data</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Hora Início</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Hora Fim</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Registro de Auto Controle - Art Coating</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>7/17/24</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Sistema de ordens de serviço de manutenção</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>7/17/24</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Sistema ICAN</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>7/17/24</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Funções no controllers para cálculos de resumo
</commit_message>
<xml_diff>
--- a/BD_TaskTick.xlsx
+++ b/BD_TaskTick.xlsx
@@ -471,31 +471,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="38.33203125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="36.5546875" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="27.88671875" bestFit="1" customWidth="1" min="3" max="3"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Projeto</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Descrição</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Cliente</t>
         </is>
@@ -583,6 +578,40 @@
       <c r="C6" t="inlineStr">
         <is>
           <t>sfdfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Sistema de inventário</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>fdjfskjdfh</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Tuopu</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>gdfgdfg</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>dfggdg</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>dfgdggd</t>
         </is>
       </c>
     </row>
@@ -597,7 +626,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -715,6 +744,50 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Sistema de ordens de serviço de manutenção</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>7/17/24</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>01:00</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>02:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Sistema de inventário</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>7/17/24</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>